<commit_message>
[Test] Add Excel compare tool
</commit_message>
<xml_diff>
--- a/员工手册.xlsx
+++ b/员工手册.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forrest/Workspace/aboutGit/github-for-non-programmers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forrest/Documents/git-for-non-coders/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>工号</t>
     <rPh sb="0" eb="1">
@@ -66,6 +66,20 @@
       <t>kuai ji</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高飞飞</t>
+    <rPh sb="0" eb="1">
+      <t>gao fei fei</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engineer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
   </si>
 </sst>
 </file>
@@ -109,9 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -389,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,6 +438,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>